<commit_message>
working on Class 3
</commit_message>
<xml_diff>
--- a/resources/DimData.xlsx
+++ b/resources/DimData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t xml:space="preserve">descriptor</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">Force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Force per unit length</t>
   </si>
   <si>
     <t xml:space="preserve">f</t>
@@ -224,14 +230,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0"/>
+    <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -336,7 +343,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,7 +376,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,10 +388,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,6 +397,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,10 +421,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -456,19 +467,19 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7" t="n">
+      <c r="D2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -477,16 +488,16 @@
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="n">
+      <c r="D3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -498,16 +509,16 @@
       <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="n">
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -519,16 +530,16 @@
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11"/>
+      <c r="E5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -540,16 +551,16 @@
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7" t="n">
+      <c r="D6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -561,13 +572,13 @@
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7" t="n">
+      <c r="D7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="n">
         <v>-2</v>
       </c>
       <c r="H7" s="4"/>
@@ -582,13 +593,13 @@
       <c r="C8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="8" t="n">
         <v>-3</v>
       </c>
-      <c r="E8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7" t="n">
+      <c r="E8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="4"/>
@@ -603,13 +614,13 @@
       <c r="C9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="E9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7" t="n">
+      <c r="E9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8" t="n">
         <v>-1</v>
       </c>
       <c r="H9" s="4"/>
@@ -624,13 +635,13 @@
       <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7" t="n">
+      <c r="D10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8" t="n">
         <v>-2</v>
       </c>
       <c r="H10" s="4"/>
@@ -645,14 +656,14 @@
       <c r="C11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7" t="n">
-        <v>-1</v>
+      <c r="D11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>-2</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -664,60 +675,60 @@
         <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="n">
         <v>-1</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <v>0</v>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>-1</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="12"/>
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -727,102 +738,102 @@
         <v>37</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="7" t="n">
-        <v>-2</v>
-      </c>
-      <c r="E16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8"/>
+      <c r="D16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4"/>
+      <c r="D17" s="8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7" t="n">
-        <v>-2</v>
-      </c>
-      <c r="H18" s="13"/>
+        <v>46</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
@@ -834,16 +845,16 @@
       <c r="C20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E20" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="13"/>
+      <c r="D20" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -853,39 +864,39 @@
         <v>51</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="D21" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="7" t="n">
-        <v>-2</v>
-      </c>
-      <c r="H22" s="13"/>
+      <c r="D22" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
@@ -895,39 +906,39 @@
         <v>56</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E23" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="7" t="n">
+        <v>55</v>
+      </c>
+      <c r="D23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="H23" s="13"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13"/>
+      <c r="D24" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
@@ -939,16 +950,16 @@
       <c r="C25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H25" s="4"/>
+      <c r="D25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
@@ -960,13 +971,13 @@
       <c r="C26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="7" t="n">
+      <c r="D26" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8" t="n">
         <v>-1</v>
       </c>
       <c r="H26" s="4"/>
@@ -981,16 +992,37 @@
       <c r="C27" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="E27" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="4"/>
+      <c r="E28" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>

</xml_diff>